<commit_message>
--- sales_quarterly = atualização de despesas
</commit_message>
<xml_diff>
--- a/sales_quarterly.xlsx
+++ b/sales_quarterly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f59780d\test_git_bash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302066B5-4328-4A65-B42F-ADDB67F5A614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CF6BB6-B293-45D9-AC40-DF1B3E6B965D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,13 +154,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -447,7 +447,7 @@
   <dimension ref="B3:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L11" sqref="L10:L11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,9 +515,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="5">
-        <v>532</v>
-      </c>
+      <c r="D7" s="7"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -526,7 +524,7 @@
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>1150</v>
       </c>
       <c r="D8" s="2"/>
@@ -538,25 +536,25 @@
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <f>SUM(C4:C8)</f>
         <v>1150</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <f>SUM(D4:D8)</f>
-        <v>532</v>
-      </c>
-      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
         <f>SUM(E4:E8)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <f>SUM(F4:F8)</f>
         <v>802.19</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <f>SUM(C9:F9)</f>
-        <v>2484.19</v>
+        <v>1952.19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>